<commit_message>
CIERRE  28 AGOSTO 21
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -582,7 +582,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44432</v>
+        <v>44436</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -668,7 +668,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44432</v>
+        <v>44436</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
cierre de 4 SEPT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -37,13 +37,13 @@
     <t>CIEN   MIL   PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t>TRES MIL    PESOS 00/100 M.N.</t>
+    <t>CUATROSCIENTOS TREINTA Y TRES    PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t xml:space="preserve">JARDINERIA P.H. </t>
+    <t>PAGO DE TURNO MATUTINO  VIERNES  27 Agosto 2021</t>
   </si>
   <si>
-    <t>SR. FELIX</t>
+    <t>JUSTINA REYES LEAL</t>
   </si>
 </sst>
 </file>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44439</v>
+        <v>44443</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -669,7 +669,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +680,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>3000</v>
+        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44439</v>
+        <v>44443</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
cierre de 7 sept 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -37,13 +37,13 @@
     <t>CIEN   MIL   PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t>CUATROSCIENTOS TREINTA Y TRES    PESOS 00/100 M.N.</t>
+    <t>CINCO MIL     PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t>PAGO DE TURNO MATUTINO  VIERNES  27 Agosto 2021</t>
+    <t>PAGO DE INCENTIVO DEL MES DE AGOSTO 2021</t>
   </si>
   <si>
-    <t>JUSTINA REYES LEAL</t>
+    <t>PABLO BAEZ</t>
   </si>
 </sst>
 </file>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44443</v>
+        <v>44446</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -669,7 +669,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +680,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>433</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44443</v>
+        <v>44446</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
media dia 11 sept 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
     <t>Arq Rodolfo Higuera Velazco</t>
   </si>
   <si>
-    <t>CIEN   MIL   PESOS 00/100 M.N.</t>
-  </si>
-  <si>
     <t>CINCO MIL     PESOS 00/100 M.N.</t>
   </si>
   <si>
@@ -44,6 +41,9 @@
   </si>
   <si>
     <t>PABLO BAEZ</t>
+  </si>
+  <si>
+    <t>CIENTO CINCUENTA    MIL   PESOS 00/100 M.N.</t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,12 +594,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>100000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44446</v>
+        <v>44450</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -668,7 +668,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
@@ -685,7 +685,7 @@
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -694,7 +694,7 @@
     <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -712,7 +712,7 @@
     </row>
     <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="15"/>
     </row>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44446</v>
+        <v>44450</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
FINAL DEL 18 SEPT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -43,7 +43,7 @@
     <t>PABLO BAEZ</t>
   </si>
   <si>
-    <t>CIENTO CINCUENTA    MIL   PESOS 00/100 M.N.</t>
+    <t>CIEn    MIL   PESOS 00/100 M.N.</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +594,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>150000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
FIN DE 25 SEPT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -43,7 +43,7 @@
     <t>PABLO BAEZ</t>
   </si>
   <si>
-    <t>CIEn    MIL   PESOS 00/100 M.N.</t>
+    <t>CIENTO CINCUENTA     MIL   PESOS 00/100 M.N.</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +594,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>100000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44457</v>
+        <v>44464</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44457</v>
+        <v>44464</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE  DEL  2 OCT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -43,7 +43,7 @@
     <t>PABLO BAEZ</t>
   </si>
   <si>
-    <t>CIENTO CINCUENTA     MIL   PESOS 00/100 M.N.</t>
+    <t xml:space="preserve"> CINCUENTA     MIL   PESOS 00/100 M.N.</t>
   </si>
 </sst>
 </file>
@@ -594,7 +594,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>150000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44464</v>
+        <v>44471</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44464</v>
+        <v>44471</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
cierre del 6 oct 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -582,7 +582,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44471</v>
+        <v>44475</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -668,7 +668,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44471</v>
+        <v>44475</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 9 oCT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -582,7 +582,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44475</v>
+        <v>44478</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -668,7 +668,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44475</v>
+        <v>44478</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 16 OCT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44478</v>
+        <v>44485</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44478</v>
+        <v>44485</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE DEL 23 OCT 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44485</v>
+        <v>44492</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44485</v>
+        <v>44492</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 6 Nov 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44492</v>
+        <v>44506</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44492</v>
+        <v>44506</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 8 NOV 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -37,13 +37,13 @@
     <t>CINCO MIL     PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t>PAGO DE INCENTIVO DEL MES DE AGOSTO 2021</t>
-  </si>
-  <si>
     <t>PABLO BAEZ</t>
   </si>
   <si>
     <t xml:space="preserve"> CINCUENTA     MIL   PESOS 00/100 M.N.</t>
+  </si>
+  <si>
+    <t>PAGO DE INCENTIVO DEL MES DE OCTUBRE 2021</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -599,7 +599,7 @@
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44506</v>
+        <v>44508</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -668,8 +668,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
     <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -712,7 +712,7 @@
     </row>
     <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="15"/>
     </row>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44506</v>
+        <v>44508</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 13 Nov 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -582,7 +582,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44508</v>
+        <v>44513</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -668,7 +668,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44508</v>
+        <v>44513</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 20 NOV 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -583,7 +583,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C15" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44513</v>
+        <v>44520</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44513</v>
+        <v>44520</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 7 DIC 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <t xml:space="preserve"> CINCUENTA     MIL   PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t>PAGO DE INCENTIVO DEL MES DE OCTUBRE 2021</t>
+    <t>PAGO DE INCENTIVO DEL MES DE NOVIEMBRE  2021</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44520</v>
+        <v>44537</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -668,7 +668,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44520</v>
+        <v>44537</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 24 DIC 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -40,10 +40,10 @@
     <t>PABLO BAEZ</t>
   </si>
   <si>
-    <t xml:space="preserve"> CINCUENTA     MIL   PESOS 00/100 M.N.</t>
+    <t>PAGO DE INCENTIVO DEL MES DE NOVIEMBRE  2021</t>
   </si>
   <si>
-    <t>PAGO DE INCENTIVO DEL MES DE NOVIEMBRE  2021</t>
+    <t>SETENTA      MIL   PESOS 00/100 M.N.</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C14:C15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,12 +594,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>50000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44541</v>
+        <v>44554</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -694,7 +694,7 @@
     <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44541</v>
+        <v>44554</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 31 DIC 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -43,7 +43,7 @@
     <t>PAGO DE INCENTIVO DEL MES DE NOVIEMBRE  2021</t>
   </si>
   <si>
-    <t>SETENTA      MIL   PESOS 00/100 M.N.</t>
+    <t>CINCUENTA      MIL   PESOS 00/100 M.N.</t>
   </si>
 </sst>
 </file>
@@ -583,7 +583,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +594,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>70000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44554</v>
+        <v>44561</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44554</v>
+        <v>44561</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 7 ENE 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -40,10 +40,10 @@
     <t>PABLO BAEZ</t>
   </si>
   <si>
-    <t>PAGO DE INCENTIVO DEL MES DE NOVIEMBRE  2021</t>
+    <t>CINCUENTA      MIL   PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t>CINCUENTA      MIL   PESOS 00/100 M.N.</t>
+    <t>PAGO DE INCENTIVO DEL MES DE DICIEMBRE  2021</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -599,7 +599,7 @@
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44561</v>
+        <v>44568</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -668,8 +668,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
     <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44561</v>
+        <v>44568</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 8 ENE 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -582,8 +582,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +643,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44568</v>
+        <v>44569</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -668,7 +668,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -729,7 +729,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44568</v>
+        <v>44569</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 31 ENE 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>OBRA ESTACIONAMIENTO OBRADOR</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>CIEN    MIL   PESOS 00/100 M.N.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -605,7 +608,11 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>0</v>
@@ -643,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44583</v>
+        <v>44590</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -729,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44583</v>
+        <v>44590</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 12 FEB 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44600</v>
+        <v>44604</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -675,7 +675,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44600</v>
+        <v>44604</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 19 FEB 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44604</v>
+        <v>44611</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44604</v>
+        <v>44611</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 26 FEB 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44611</v>
+        <v>44618</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44611</v>
+        <v>44618</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
cierre 12 mar 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44625</v>
+        <v>44632</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -675,7 +675,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44625</v>
+        <v>44632</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 26 MAR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44632</v>
+        <v>44646</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44632</v>
+        <v>44646</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 2 ABRIL 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -586,7 +586,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44646</v>
+        <v>44653</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44646</v>
+        <v>44653</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 5 abr 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>PAGO DE INCENTIVO DEL MES DE FEBRERO  2022</t>
+    <t>PAGO DE INCENTIVO DEL MES DE MARZO  2022</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44653</v>
+        <v>44656</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -675,7 +675,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44653</v>
+        <v>44656</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
cierre 9 ABRIL 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44656</v>
+        <v>44660</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -675,7 +675,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44656</v>
+        <v>44660</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 30 ABR 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44667</v>
+        <v>44681</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44667</v>
+        <v>44681</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 6 MAY 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>PAGO DE INCENTIVO DEL MES DE MARZO  2022</t>
+    <t>PAGO DE INCENTIVO DEL MES DE  ABRIL   2022</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44681</v>
+        <v>44687</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -675,7 +675,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44681</v>
+        <v>44687</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 14 MAY 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:D5"/>
     </sheetView>
   </sheetViews>
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44687</v>
+        <v>44695</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -675,7 +675,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44687</v>
+        <v>44695</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 21 MAY 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -586,7 +586,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D5"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44695</v>
+        <v>44702</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44695</v>
+        <v>44702</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE  4 JUN 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -43,10 +43,10 @@
     <t>PAGO DE INCENTIVO DEL MES DE  ABRIL   2022</t>
   </si>
   <si>
-    <t>CINCUENTA    MIL   PESOS 00/100 M.N.</t>
+    <t>CIENTO CINCUENTA    MIL   PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t xml:space="preserve">PAGO SOBRE DEMOLICION DE  11 SUR </t>
+    <t xml:space="preserve">OBRA ESTACIONAMIENTO OBRADOR </t>
   </si>
 </sst>
 </file>
@@ -586,7 +586,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +597,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>50000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -650,7 +650,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44709</v>
+        <v>44716</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -736,7 +736,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44709</v>
+        <v>44716</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 8 JUN 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -34,19 +34,19 @@
     <t>CINCO MIL     PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t>PABLO BAEZ</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
-  </si>
-  <si>
-    <t>PAGO DE INCENTIVO DEL MES DE  ABRIL   2022</t>
   </si>
   <si>
     <t>CIENTO CINCUENTA    MIL   PESOS 00/100 M.N.</t>
   </si>
   <si>
     <t xml:space="preserve">OBRA ESTACIONAMIENTO OBRADOR </t>
+  </si>
+  <si>
+    <t>PAGO DE INCENTIVO DEL MES DE  MAYO   2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                           PABLO BAEZ</t>
   </si>
 </sst>
 </file>
@@ -250,7 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,6 +298,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -585,7 +597,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -602,7 +614,7 @@
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -610,12 +622,12 @@
     </row>
     <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -650,7 +662,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44716</v>
+        <v>44720</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -675,8 +687,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +713,7 @@
     <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -718,14 +730,14 @@
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="15"/>
+      <c r="C8" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="19"/>
     </row>
     <row r="9" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
@@ -736,7 +748,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44716</v>
+        <v>44720</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
cierre 10 Jun 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -597,13 +597,14 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -662,7 +663,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44720</v>
+        <v>44722</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -687,13 +688,14 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -748,7 +750,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44720</v>
+        <v>44722</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 11 JUN 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -37,9 +37,6 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>CIENTO CINCUENTA    MIL   PESOS 00/100 M.N.</t>
-  </si>
-  <si>
     <t xml:space="preserve">OBRA ESTACIONAMIENTO OBRADOR </t>
   </si>
   <si>
@@ -47,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">                           PABLO BAEZ</t>
+  </si>
+  <si>
+    <t>CIENTO    MIL   PESOS 00/100 M.N.</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,12 +610,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>150000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -628,7 +628,7 @@
     </row>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -663,7 +663,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44722</v>
+        <v>44723</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -715,7 +715,7 @@
     <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -733,7 +733,7 @@
     </row>
     <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="19"/>
     </row>
@@ -750,7 +750,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44722</v>
+        <v>44723</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
cierre 18 Jun 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">                           PABLO BAEZ</t>
   </si>
   <si>
-    <t>CIENTO    MIL   PESOS 00/100 M.N.</t>
+    <t>CIEN    MIL   PESOS 00/100 M.N.</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +610,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>50000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -663,7 +663,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44723</v>
+        <v>44730</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -750,7 +750,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44723</v>
+        <v>44730</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 6 JUL 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -40,13 +40,13 @@
     <t xml:space="preserve">OBRA ESTACIONAMIENTO OBRADOR </t>
   </si>
   <si>
-    <t>PAGO DE INCENTIVO DEL MES DE  MAYO   2022</t>
-  </si>
-  <si>
     <t xml:space="preserve">                           PABLO BAEZ</t>
   </si>
   <si>
     <t>CIEN    MIL   PESOS 00/100 M.N.</t>
+  </si>
+  <si>
+    <t>PAGO DE INCENTIVO DEL MES DE  JUNIO   2022</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
@@ -615,7 +615,7 @@
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -663,7 +663,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44730</v>
+        <v>44748</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -688,8 +688,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +715,7 @@
     <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -733,7 +733,7 @@
     </row>
     <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="19"/>
     </row>
@@ -750,7 +750,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44730</v>
+        <v>44748</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 11 JUL 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -597,7 +597,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
@@ -663,7 +663,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44748</v>
+        <v>44751</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -688,7 +688,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -750,7 +750,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44748</v>
+        <v>44751</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
cierre 16 Julio 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -663,7 +663,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44751</v>
+        <v>44758</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -750,7 +750,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44751</v>
+        <v>44758</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE  13 Ago 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -651,7 +651,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44779</v>
+        <v>44786</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -738,7 +738,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44779</v>
+        <v>44786</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 3 SEPT 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -651,7 +651,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44786</v>
+        <v>44807</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -738,7 +738,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44786</v>
+        <v>44807</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 7 SEPT 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -40,13 +40,13 @@
     <t xml:space="preserve">                           PABLO BAEZ</t>
   </si>
   <si>
-    <t>PAGO DE INCENTIVO DEL MES DE  JUNIO   2022</t>
-  </si>
-  <si>
     <t>CIEN   MIL   PESOS 00/100 M.N.</t>
   </si>
   <si>
     <t>Arq Rodolfo Higuera Velazco</t>
+  </si>
+  <si>
+    <t>PAGO DE INCENTIVO DEL MES DE  AGOSTO   2022</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +603,7 @@
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -634,7 +634,7 @@
     </row>
     <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8" s="15"/>
     </row>
@@ -651,7 +651,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44807</v>
+        <v>44811</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -676,7 +676,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -703,7 +703,7 @@
     <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -738,7 +738,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44807</v>
+        <v>44811</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE  10 SEPT 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -651,7 +651,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44811</v>
+        <v>44814</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -676,7 +676,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -738,7 +738,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44811</v>
+        <v>44814</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 17 SEPT 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -651,7 +651,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44814</v>
+        <v>44821</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -738,7 +738,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44814</v>
+        <v>44821</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 6 OCT 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <t>Arq Rodolfo Higuera Velazco</t>
   </si>
   <si>
-    <t>PAGO DE INCENTIVO DEL MES DE  AGOSTO   2022</t>
+    <t>PAGO DE INCENTIVO DEL MES DE  SEPTIEMBRE   2022</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -651,7 +651,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44821</v>
+        <v>44840</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -676,7 +676,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -738,7 +738,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44821</v>
+        <v>44840</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
cierre 28 Dic- 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t xml:space="preserve">  </t>
   </si>
@@ -37,16 +37,16 @@
     <t xml:space="preserve">OBRA ESTACIONAMIENTO OBRADOR </t>
   </si>
   <si>
-    <t>CINCO MIL    PESOS 00/100 M.N.</t>
+    <t>DIECIOCHO  MIL  SETECIENTOS SESENTA     PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t>INCENTIVO DEL MES DE ______</t>
+    <t>CINCO   MIL     PESOS 00/100 M.N.</t>
   </si>
   <si>
     <t>PABLO BAEZ</t>
   </si>
   <si>
-    <t>DIECIOCHO  MIL  SETECIENTOS SESENTA     PESOS 00/100 M.N.</t>
+    <t>INCENTIVO DEL MES DE NOVIEMBRE</t>
   </si>
 </sst>
 </file>
@@ -585,8 +585,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +603,7 @@
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -651,7 +651,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44921</v>
+        <v>44923</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -676,14 +676,14 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -694,16 +694,20 @@
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -738,7 +742,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44921</v>
+        <v>44923</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -747,9 +751,9 @@
   <mergeCells count="5">
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A4:D5"/>
-    <mergeCell ref="C8:D9"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C8:D9"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.35433070866141736" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
cierre 30 Dic 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t xml:space="preserve">OBRA ESTACIONAMIENTO OBRADOR </t>
   </si>
   <si>
-    <t>DIECIOCHO  MIL  SETECIENTOS SESENTA     PESOS 00/100 M.N.</t>
-  </si>
-  <si>
     <t>CINCO   MIL     PESOS 00/100 M.N.</t>
   </si>
   <si>
@@ -47,6 +44,9 @@
   </si>
   <si>
     <t>INCENTIVO DEL MES DE NOVIEMBRE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   TREINTA   MIL      PESOS 00/100 M.N.</t>
   </si>
 </sst>
 </file>
@@ -585,8 +585,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,12 +598,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>18760</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -651,7 +651,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44923</v>
+        <v>44925</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -676,7 +676,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -694,7 +694,7 @@
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -707,7 +707,7 @@
     </row>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -725,7 +725,7 @@
     </row>
     <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="15"/>
     </row>
@@ -742,7 +742,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>44923</v>
+        <v>44925</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 22 JUL 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -702,7 +702,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45115</v>
+        <v>45129</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -793,7 +793,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45115</v>
+        <v>45129</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
cierre 29- jul 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -702,7 +702,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45135</v>
+        <v>45136</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -793,7 +793,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45135</v>
+        <v>45136</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 11 AGO 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -31,9 +31,6 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>CINCO   MIL     PESOS 00/100 M.N.</t>
-  </si>
-  <si>
     <t>PABLO BAEZ</t>
   </si>
   <si>
@@ -46,7 +43,10 @@
     <t>PAGO TRABAJOS AMPLIACION DE OBRADOR</t>
   </si>
   <si>
-    <t>INCENTIVO DEL MES DE  JUNIO     2023</t>
+    <t>SEIS   MIL     PESOS 00/100 M.N.</t>
+  </si>
+  <si>
+    <t>INCENTIVO DEL MES DE  JULIO     2023</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -648,7 +648,7 @@
     </row>
     <row r="2" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -661,7 +661,7 @@
     </row>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -685,7 +685,7 @@
     </row>
     <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="9"/>
     </row>
@@ -702,7 +702,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45143</v>
+        <v>45149</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -727,8 +727,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,12 +740,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>5000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -776,7 +776,7 @@
     </row>
     <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="9"/>
     </row>
@@ -793,7 +793,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45143</v>
+        <v>45149</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 26- AGO 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -34,19 +34,19 @@
     <t>PABLO BAEZ</t>
   </si>
   <si>
-    <t>CIEN     MIL        PESOS 00/100 M.N.</t>
+    <t>SEIS   MIL     PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t>Arq.Rodolfo Higuera Vezazco</t>
+    <t>INCENTIVO DEL MES DE  JULIO     2023</t>
+  </si>
+  <si>
+    <t>CIEN   MIL        PESOS 00/100 M.N.</t>
   </si>
   <si>
     <t>PAGO TRABAJOS AMPLIACION DE OBRADOR</t>
   </si>
   <si>
-    <t>SEIS   MIL     PESOS 00/100 M.N.</t>
-  </si>
-  <si>
-    <t>INCENTIVO DEL MES DE  JULIO     2023</t>
+    <t>Arq. Rodolfo Higuera Velazco</t>
   </si>
 </sst>
 </file>
@@ -631,7 +631,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +648,7 @@
     </row>
     <row r="2" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -661,7 +661,7 @@
     </row>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -685,7 +685,7 @@
     </row>
     <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D8" s="9"/>
     </row>
@@ -702,7 +702,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45157</v>
+        <v>45164</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -745,7 +745,7 @@
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -758,7 +758,7 @@
     </row>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -793,7 +793,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45157</v>
+        <v>45164</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 18 Sep 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -702,7 +702,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45184</v>
+        <v>45188</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -793,7 +793,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45184</v>
+        <v>45188</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
cierre 25- sept 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -702,7 +702,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45188</v>
+        <v>45194</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -793,7 +793,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45188</v>
+        <v>45194</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
cierre 31 oct 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -702,7 +702,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45222</v>
+        <v>45230</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -793,7 +793,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45222</v>
+        <v>45230</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 27 NOV 2023
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -40,10 +40,10 @@
     <t xml:space="preserve">AMPLIACION REMODELACION DE   11 SUR  </t>
   </si>
   <si>
-    <t>SEIS  MIL   PESOS 08/100 M.N.</t>
+    <t>PAGO DE INCENTIVO PABLO BAEZ  OCTUBRE 2023</t>
   </si>
   <si>
-    <t>PAGO DE INCENTIVO PABLO BAEZ  OCTUBRE 2023</t>
+    <t>SEIS  MIL   PESOS 00/100 M.N.</t>
   </si>
 </sst>
 </file>
@@ -627,7 +627,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -699,7 +699,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45254</v>
+        <v>45257</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -724,8 +724,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +742,7 @@
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -755,7 +755,7 @@
     </row>
     <row r="4" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -788,7 +788,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45254</v>
+        <v>45257</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 11 DIC 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -627,7 +627,7 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -699,7 +699,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45267</v>
+        <v>45271</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -724,8 +724,8 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,7 +788,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45267</v>
+        <v>45271</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 18 DIC 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -699,7 +699,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45271</v>
+        <v>45278</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -788,7 +788,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45271</v>
+        <v>45278</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
CIERRE 26 DIC 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -40,13 +40,13 @@
     <t xml:space="preserve">AMPLIACION REMODELACION DE   11 SUR  </t>
   </si>
   <si>
-    <t>CINCO  MIL   PESOS 00/100 M.N.</t>
+    <t>SEIS  MIL   PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t xml:space="preserve">COMPLEMENTO DE SUELDO VIAJE 20-Dic-23 RES Guadalajara Y Viernes 22-Dic-23 FYRASA  </t>
+    <t xml:space="preserve">INCENTIVO DEL MES DE  NOVIEMBRRE 2023   </t>
   </si>
   <si>
-    <t>ARTURO AGUILAR  DIAZ</t>
+    <t>PABLO BAEZ</t>
   </si>
 </sst>
 </file>
@@ -702,7 +702,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45283</v>
+        <v>45286</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>
@@ -740,7 +740,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="2">
-        <v>5000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -793,7 +793,7 @@
     <row r="11" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <f ca="1">TODAY()</f>
-        <v>45283</v>
+        <v>45286</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
VIERNES 10 MAYO 2024
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/AAB  V A L E S.xlsx
+++ b/01 DOCUEMENTOS/AAB  V A L E S.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620"/>
+    <workbookView xWindow="11280" yWindow="1845" windowWidth="17085" windowHeight="13620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARQUITECTO        " sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <t>CIEN   MIL       PESOS 00/100 M.N.</t>
   </si>
   <si>
-    <t>INCENTIVO DEL MES DE  MARZO   2024</t>
+    <t>INCENTIVO DEL MES DE  ABRIL   2024</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -705,7 +705,7 @@
     <row r="12" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <f ca="1">TODAY()</f>
-        <v>45418</v>
+        <v>45422</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="1"/>
@@ -730,8 +730,8 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +799,7 @@
     <row r="12" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <f ca="1">TODAY()</f>
-        <v>45418</v>
+        <v>45422</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="1"/>

</xml_diff>